<commit_message>
Bug fixes and refactoring
</commit_message>
<xml_diff>
--- a/sample_data/pickup_items_rough.xlsx
+++ b/sample_data/pickup_items_rough.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihir\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mihir\Projects\warehouse-delivery-optimization\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11782B94-C246-48C7-9EFC-48D5A387BF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58CB6C1-1345-4461-B144-6C891B815B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>name</t>
   </si>
@@ -55,15 +55,6 @@
     <t>warehouse</t>
   </si>
   <si>
-    <t>Pickup Addr 1</t>
-  </si>
-  <si>
-    <t>Pickup Addr 2</t>
-  </si>
-  <si>
-    <t>Pickup Addr 3</t>
-  </si>
-  <si>
     <t>sfq2234</t>
   </si>
   <si>
@@ -73,15 +64,6 @@
     <t>4sgw3</t>
   </si>
   <si>
-    <t>2025-08-03T04:46:38.426Z</t>
-  </si>
-  <si>
-    <t>2025-08-08T15:44:38.426Z</t>
-  </si>
-  <si>
-    <t>2025-08-06T07:55:38.426Z</t>
-  </si>
-  <si>
     <t>Pickup Item 1 Desc</t>
   </si>
   <si>
@@ -98,6 +80,30 @@
   </si>
   <si>
     <t>Pickup Item 3</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>2025-08-03T14:06:38.426+00:00</t>
+  </si>
+  <si>
+    <t>2025-08-06T15:05:38.426+00:00</t>
+  </si>
+  <si>
+    <t>2025-08-06T16:07:38.426+00:00</t>
+  </si>
+  <si>
+    <t>Prost</t>
+  </si>
+  <si>
+    <t>Serai</t>
+  </si>
+  <si>
+    <t>Birla</t>
   </si>
 </sst>
 </file>
@@ -474,16 +480,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
@@ -492,7 +499,7 @@
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,105 +530,130 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="F2">
-        <v>143</v>
+        <v>17.4297545716854</v>
       </c>
       <c r="G2">
-        <v>34</v>
+        <v>78.402998253527599</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
       </c>
       <c r="I2">
-        <v>10</v>
+        <v>17.405991509704702</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>78.403749492154006</v>
+      </c>
+      <c r="K2">
+        <v>3.64</v>
+      </c>
+      <c r="L2">
+        <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F3">
-        <v>123</v>
+        <v>17.442972009170301</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>78.382623222841602</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
       <c r="I3">
-        <v>10</v>
+        <v>17.405991509704702</v>
       </c>
       <c r="J3">
-        <v>10</v>
+        <v>78.403749492154006</v>
+      </c>
+      <c r="K3">
+        <v>6.32</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="F4">
-        <v>25</v>
+        <v>17.406451671598401</v>
       </c>
       <c r="G4">
-        <v>76</v>
+        <v>78.469285399556597</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
       <c r="I4">
-        <v>10</v>
+        <v>17.405991509704702</v>
       </c>
       <c r="J4">
-        <v>10</v>
+        <v>78.403749492154006</v>
+      </c>
+      <c r="K4">
+        <v>5.13</v>
+      </c>
+      <c r="L4">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:J1" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>